<commit_message>
template download + import pro services from csv ok
</commit_message>
<xml_diff>
--- a/app/import_clients_template.xlsx
+++ b/app/import_clients_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\Firestore-PHP\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1389B43-456D-4632-8037-71F004046FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB6507A-678C-4C54-86F5-97302A3F2BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>first_name_1</t>
   </si>
@@ -65,65 +65,17 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>nidhal</t>
-  </si>
-  <si>
-    <t>sfr</t>
-  </si>
-  <si>
-    <t>14 street tyr</t>
-  </si>
-  <si>
-    <t>megrine</t>
-  </si>
-  <si>
-    <t>ben arous</t>
-  </si>
-  <si>
-    <t>type test</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>nid@aol.com</t>
-  </si>
-  <si>
-    <t>0021627119042</t>
-  </si>
-  <si>
-    <t>ouss@test.com</t>
-  </si>
-  <si>
-    <t>0021612345678</t>
-  </si>
-  <si>
-    <t>test notes</t>
-  </si>
-  <si>
-    <t>Oussema</t>
-  </si>
-  <si>
-    <t>Sferi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -132,13 +84,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,30 +103,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,131 +425,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.19921875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.09765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="1"/>
-    <col min="8" max="8" width="13.296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.296875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="9.8984375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" style="1"/>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.296875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.09765625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" style="4"/>
+    <col min="8" max="8" width="13.296875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.796875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.296875" style="4" customWidth="1"/>
+    <col min="11" max="12" width="9.8984375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" style="4"/>
+    <col min="14" max="14" width="13.5" style="5" customWidth="1"/>
+    <col min="15" max="15" width="11.19921875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="3">
-        <v>2024</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{4E4AF66E-99E7-4726-BFEF-ABCC9582884A}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{10853FF1-2362-48C3-9F30-19AFFC3B724B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;8&amp;K000000 Restricted Access&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>